<commit_message>
Actualizado a la ultima version
</commit_message>
<xml_diff>
--- a/normativa/Anexos/L05T02C03/L05T02C03A04_27.xlsx
+++ b/normativa/Anexos/L05T02C03/L05T02C03A04_27.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" tabRatio="663" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4710" tabRatio="663" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="HOJA 2" sheetId="2" state="hidden" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="3">'Anexo 4.27C'!$A$1:$G$42</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'Anexo 4.27D'!$A$1:$G$39</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">'Anexo 4.27E'!$A$1:$H$39</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="6">'Anexo 4.27F'!$A$1:$H$71</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">'Anexo 4.27F'!$A$1:$H$74</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'HOJA 2'!$A$1:$L$65</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="6">'Anexo 4.27F'!$1:$11</definedName>
   </definedNames>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="178">
   <si>
     <t>Contador General</t>
   </si>
@@ -664,13 +664,38 @@
     <t>Cuentas de orden contigentes acreedoras</t>
   </si>
   <si>
-    <t xml:space="preserve">  (**)   Se considera a los Fondos de Garantía de Créditos para el Sector Productivo, de Vivienda de Interés Social y para el Sector Gremial, a efectos de validar la integridad de la información financiera.</t>
+    <t>975.00</t>
+  </si>
+  <si>
+    <t>976.00</t>
+  </si>
+  <si>
+    <t>Obligaciones privilegiadas de segundo orden</t>
+  </si>
+  <si>
+    <t>Obligaciones privilegiadas de primer orden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            la integridad de la información financiera.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  (**)   Se considera a los Fondos de Garantía de Créditos para el Sector Productivo, de Vivienda de Interés Social, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>para el Sector Gremial y del Fondo de Garantía de Apoyo a la Construcción, a efectos de validar</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1042,7 +1067,7 @@
     <xf numFmtId="39" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="39" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1306,14 +1331,17 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="39" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="39" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1324,6 +1352,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF3333FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1336,7 +1369,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1628,7 +1661,7 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="3.7109375" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" style="1" customWidth="1"/>
     <col min="2" max="3" width="22.5703125" style="1" customWidth="1"/>
@@ -3717,11 +3750,9 @@
   </sheetPr>
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
-    </sheetView>
+    <sheetView view="pageBreakPreview" topLeftCell="A31" zoomScale="90" zoomScaleNormal="115" zoomScaleSheetLayoutView="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="3.7109375" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" style="36" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" style="36" customWidth="1"/>
@@ -4402,11 +4433,9 @@
   </sheetPr>
   <dimension ref="A1:T58"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
-    </sheetView>
+    <sheetView topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.85546875" style="36" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" style="36"/>
@@ -5386,11 +5415,9 @@
   </sheetPr>
   <dimension ref="A1:AL55"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:A33"/>
-    </sheetView>
+    <sheetView topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="3.7109375" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.140625" style="36" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" style="36" customWidth="1"/>
@@ -6257,11 +6284,9 @@
   </sheetPr>
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:G29"/>
-    </sheetView>
+    <sheetView topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.85546875" style="36" customWidth="1"/>
     <col min="2" max="2" width="25.42578125" style="36" customWidth="1"/>
@@ -6728,11 +6753,9 @@
   </sheetPr>
   <dimension ref="A1:AL54"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
-    </sheetView>
+    <sheetView topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="3.7109375" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.85546875" style="36" customWidth="1"/>
     <col min="2" max="2" width="32.85546875" style="36" customWidth="1"/>
@@ -7490,13 +7513,13 @@
     <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AL86"/>
+  <dimension ref="A1:AL89"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A40" zoomScaleNormal="100" zoomScaleSheetLayoutView="120" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="90" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66:H66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="3.7109375" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.140625" style="36" customWidth="1"/>
     <col min="2" max="2" width="53.85546875" style="36" customWidth="1"/>
@@ -8089,9 +8112,13 @@
       <c r="G27" s="65"/>
       <c r="H27" s="65"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="91"/>
-      <c r="B28" s="65"/>
+    <row r="28" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="91" t="s">
+        <v>172</v>
+      </c>
+      <c r="B28" s="65" t="s">
+        <v>175</v>
+      </c>
       <c r="C28" s="65"/>
       <c r="D28" s="65"/>
       <c r="E28" s="65"/>
@@ -8099,12 +8126,12 @@
       <c r="G28" s="65"/>
       <c r="H28" s="65"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="91" t="s">
-        <v>134</v>
+        <v>173</v>
       </c>
       <c r="B29" s="65" t="s">
-        <v>48</v>
+        <v>174</v>
       </c>
       <c r="C29" s="65"/>
       <c r="D29" s="65"/>
@@ -8114,12 +8141,8 @@
       <c r="H29" s="65"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="91" t="s">
-        <v>135</v>
-      </c>
-      <c r="B30" s="65" t="s">
-        <v>49</v>
-      </c>
+      <c r="A30" s="91"/>
+      <c r="B30" s="65"/>
       <c r="C30" s="65"/>
       <c r="D30" s="65"/>
       <c r="E30" s="65"/>
@@ -8128,8 +8151,12 @@
       <c r="H30" s="65"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="91"/>
-      <c r="B31" s="65"/>
+      <c r="A31" s="91" t="s">
+        <v>134</v>
+      </c>
+      <c r="B31" s="65" t="s">
+        <v>48</v>
+      </c>
       <c r="C31" s="65"/>
       <c r="D31" s="65"/>
       <c r="E31" s="65"/>
@@ -8138,9 +8165,11 @@
       <c r="H31" s="65"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="91"/>
-      <c r="B32" s="92" t="s">
-        <v>45</v>
+      <c r="A32" s="91" t="s">
+        <v>135</v>
+      </c>
+      <c r="B32" s="65" t="s">
+        <v>49</v>
       </c>
       <c r="C32" s="65"/>
       <c r="D32" s="65"/>
@@ -8150,12 +8179,8 @@
       <c r="H32" s="65"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="91" t="s">
-        <v>136</v>
-      </c>
-      <c r="B33" s="65" t="s">
-        <v>137</v>
-      </c>
+      <c r="A33" s="91"/>
+      <c r="B33" s="65"/>
       <c r="C33" s="65"/>
       <c r="D33" s="65"/>
       <c r="E33" s="65"/>
@@ -8164,11 +8189,9 @@
       <c r="H33" s="65"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="91" t="s">
-        <v>138</v>
-      </c>
-      <c r="B34" s="65" t="s">
-        <v>34</v>
+      <c r="A34" s="91"/>
+      <c r="B34" s="92" t="s">
+        <v>45</v>
       </c>
       <c r="C34" s="65"/>
       <c r="D34" s="65"/>
@@ -8178,9 +8201,11 @@
       <c r="H34" s="65"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="93"/>
+      <c r="A35" s="91" t="s">
+        <v>136</v>
+      </c>
       <c r="B35" s="65" t="s">
-        <v>47</v>
+        <v>137</v>
       </c>
       <c r="C35" s="65"/>
       <c r="D35" s="65"/>
@@ -8190,8 +8215,12 @@
       <c r="H35" s="65"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="93"/>
-      <c r="B36" s="65"/>
+      <c r="A36" s="91" t="s">
+        <v>138</v>
+      </c>
+      <c r="B36" s="65" t="s">
+        <v>34</v>
+      </c>
       <c r="C36" s="65"/>
       <c r="D36" s="65"/>
       <c r="E36" s="65"/>
@@ -8200,61 +8229,55 @@
       <c r="H36" s="65"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="121" t="s">
+      <c r="A37" s="93"/>
+      <c r="B37" s="65" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" s="65"/>
+      <c r="D37" s="65"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="65"/>
+      <c r="G37" s="65"/>
+      <c r="H37" s="65"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="93"/>
+      <c r="B38" s="65"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="65"/>
+      <c r="E38" s="65"/>
+      <c r="F38" s="65"/>
+      <c r="G38" s="65"/>
+      <c r="H38" s="65"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="121" t="s">
         <v>51</v>
       </c>
-      <c r="B37" s="122"/>
-      <c r="C37" s="122"/>
-      <c r="D37" s="122"/>
-      <c r="E37" s="122"/>
-      <c r="F37" s="122"/>
-      <c r="G37" s="122"/>
-      <c r="H37" s="123"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="88"/>
-      <c r="B38" s="89" t="s">
+      <c r="B39" s="122"/>
+      <c r="C39" s="122"/>
+      <c r="D39" s="122"/>
+      <c r="E39" s="122"/>
+      <c r="F39" s="122"/>
+      <c r="G39" s="122"/>
+      <c r="H39" s="123"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="88"/>
+      <c r="B40" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="C38" s="90"/>
-      <c r="D38" s="90"/>
-      <c r="E38" s="90"/>
-      <c r="F38" s="90"/>
-      <c r="G38" s="90"/>
-      <c r="H38" s="90"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="91"/>
-      <c r="B39" s="92" t="s">
+      <c r="C40" s="90"/>
+      <c r="D40" s="90"/>
+      <c r="E40" s="90"/>
+      <c r="F40" s="90"/>
+      <c r="G40" s="90"/>
+      <c r="H40" s="90"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="91"/>
+      <c r="B41" s="92" t="s">
         <v>55</v>
-      </c>
-      <c r="C39" s="65"/>
-      <c r="D39" s="65"/>
-      <c r="E39" s="65"/>
-      <c r="F39" s="65"/>
-      <c r="G39" s="65"/>
-      <c r="H39" s="65"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="91" t="s">
-        <v>139</v>
-      </c>
-      <c r="B40" s="65" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" s="65"/>
-      <c r="D40" s="65"/>
-      <c r="E40" s="65"/>
-      <c r="F40" s="65"/>
-      <c r="G40" s="65"/>
-      <c r="H40" s="65"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="91" t="s">
-        <v>140</v>
-      </c>
-      <c r="B41" s="65" t="s">
-        <v>36</v>
       </c>
       <c r="C41" s="65"/>
       <c r="D41" s="65"/>
@@ -8265,10 +8288,10 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="91" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B42" s="65" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C42" s="65"/>
       <c r="D42" s="65"/>
@@ -8279,10 +8302,10 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="91" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B43" s="65" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C43" s="65"/>
       <c r="D43" s="65"/>
@@ -8293,10 +8316,10 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="91" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B44" s="65" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C44" s="65"/>
       <c r="D44" s="65"/>
@@ -8307,10 +8330,10 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="91" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B45" s="65" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C45" s="65"/>
       <c r="D45" s="65"/>
@@ -8321,10 +8344,10 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="91" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B46" s="65" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C46" s="65"/>
       <c r="D46" s="65"/>
@@ -8335,10 +8358,10 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="91" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B47" s="65" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C47" s="65"/>
       <c r="D47" s="65"/>
@@ -8348,8 +8371,12 @@
       <c r="H47" s="65"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="91"/>
-      <c r="B48" s="65"/>
+      <c r="A48" s="91" t="s">
+        <v>145</v>
+      </c>
+      <c r="B48" s="65" t="s">
+        <v>32</v>
+      </c>
       <c r="C48" s="65"/>
       <c r="D48" s="65"/>
       <c r="E48" s="65"/>
@@ -8357,10 +8384,12 @@
       <c r="G48" s="65"/>
       <c r="H48" s="65"/>
     </row>
-    <row r="49" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A49" s="91"/>
-      <c r="B49" s="92" t="s">
-        <v>56</v>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="91" t="s">
+        <v>146</v>
+      </c>
+      <c r="B49" s="65" t="s">
+        <v>33</v>
       </c>
       <c r="C49" s="65"/>
       <c r="D49" s="65"/>
@@ -8369,13 +8398,9 @@
       <c r="G49" s="65"/>
       <c r="H49" s="65"/>
     </row>
-    <row r="50" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A50" s="91" t="s">
-        <v>147</v>
-      </c>
-      <c r="B50" s="65" t="s">
-        <v>52</v>
-      </c>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="91"/>
+      <c r="B50" s="65"/>
       <c r="C50" s="65"/>
       <c r="D50" s="65"/>
       <c r="E50" s="65"/>
@@ -8383,12 +8408,10 @@
       <c r="G50" s="65"/>
       <c r="H50" s="65"/>
     </row>
-    <row r="51" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A51" s="91" t="s">
-        <v>148</v>
-      </c>
-      <c r="B51" s="65" t="s">
-        <v>41</v>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="91"/>
+      <c r="B51" s="92" t="s">
+        <v>56</v>
       </c>
       <c r="C51" s="65"/>
       <c r="D51" s="65"/>
@@ -8397,12 +8420,12 @@
       <c r="G51" s="65"/>
       <c r="H51" s="65"/>
     </row>
-    <row r="52" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="91" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B52" s="65" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C52" s="65"/>
       <c r="D52" s="65"/>
@@ -8411,9 +8434,13 @@
       <c r="G52" s="65"/>
       <c r="H52" s="65"/>
     </row>
-    <row r="53" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A53" s="91"/>
-      <c r="B53" s="65"/>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="91" t="s">
+        <v>148</v>
+      </c>
+      <c r="B53" s="65" t="s">
+        <v>41</v>
+      </c>
       <c r="C53" s="65"/>
       <c r="D53" s="65"/>
       <c r="E53" s="65"/>
@@ -8421,12 +8448,12 @@
       <c r="G53" s="65"/>
       <c r="H53" s="65"/>
     </row>
-    <row r="54" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A54" s="91">
-        <v>988</v>
-      </c>
-      <c r="B54" s="100" t="s">
-        <v>171</v>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="91" t="s">
+        <v>149</v>
+      </c>
+      <c r="B54" s="65" t="s">
+        <v>42</v>
       </c>
       <c r="C54" s="65"/>
       <c r="D54" s="65"/>
@@ -8435,13 +8462,9 @@
       <c r="G54" s="65"/>
       <c r="H54" s="65"/>
     </row>
-    <row r="55" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A55" s="91" t="s">
-        <v>150</v>
-      </c>
-      <c r="B55" s="65" t="s">
-        <v>49</v>
-      </c>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="91"/>
+      <c r="B55" s="65"/>
       <c r="C55" s="65"/>
       <c r="D55" s="65"/>
       <c r="E55" s="65"/>
@@ -8449,9 +8472,13 @@
       <c r="G55" s="65"/>
       <c r="H55" s="65"/>
     </row>
-    <row r="56" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A56" s="91"/>
-      <c r="B56" s="65"/>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="91">
+        <v>988</v>
+      </c>
+      <c r="B56" s="100" t="s">
+        <v>171</v>
+      </c>
       <c r="C56" s="65"/>
       <c r="D56" s="65"/>
       <c r="E56" s="65"/>
@@ -8459,10 +8486,12 @@
       <c r="G56" s="65"/>
       <c r="H56" s="65"/>
     </row>
-    <row r="57" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A57" s="91"/>
-      <c r="B57" s="92" t="s">
-        <v>45</v>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="91" t="s">
+        <v>150</v>
+      </c>
+      <c r="B57" s="65" t="s">
+        <v>49</v>
       </c>
       <c r="C57" s="65"/>
       <c r="D57" s="65"/>
@@ -8471,13 +8500,9 @@
       <c r="G57" s="65"/>
       <c r="H57" s="65"/>
     </row>
-    <row r="58" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A58" s="91" t="s">
-        <v>151</v>
-      </c>
-      <c r="B58" s="65" t="s">
-        <v>137</v>
-      </c>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="91"/>
+      <c r="B58" s="65"/>
       <c r="C58" s="65"/>
       <c r="D58" s="65"/>
       <c r="E58" s="65"/>
@@ -8485,12 +8510,10 @@
       <c r="G58" s="65"/>
       <c r="H58" s="65"/>
     </row>
-    <row r="59" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A59" s="91" t="s">
-        <v>152</v>
-      </c>
-      <c r="B59" s="65" t="s">
-        <v>34</v>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="91"/>
+      <c r="B59" s="92" t="s">
+        <v>45</v>
       </c>
       <c r="C59" s="65"/>
       <c r="D59" s="65"/>
@@ -8499,10 +8522,12 @@
       <c r="G59" s="65"/>
       <c r="H59" s="65"/>
     </row>
-    <row r="60" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A60" s="93"/>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="91" t="s">
+        <v>151</v>
+      </c>
       <c r="B60" s="65" t="s">
-        <v>47</v>
+        <v>137</v>
       </c>
       <c r="C60" s="65"/>
       <c r="D60" s="65"/>
@@ -8511,191 +8536,204 @@
       <c r="G60" s="65"/>
       <c r="H60" s="65"/>
     </row>
-    <row r="61" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A61" s="119" t="s">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="91" t="s">
+        <v>152</v>
+      </c>
+      <c r="B61" s="65" t="s">
+        <v>34</v>
+      </c>
+      <c r="C61" s="65"/>
+      <c r="D61" s="65"/>
+      <c r="E61" s="65"/>
+      <c r="F61" s="65"/>
+      <c r="G61" s="65"/>
+      <c r="H61" s="65"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="93"/>
+      <c r="B62" s="65" t="s">
+        <v>47</v>
+      </c>
+      <c r="C62" s="65"/>
+      <c r="D62" s="65"/>
+      <c r="E62" s="65"/>
+      <c r="F62" s="65"/>
+      <c r="G62" s="65"/>
+      <c r="H62" s="65"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="B61" s="120"/>
-      <c r="C61" s="94"/>
-      <c r="D61" s="94"/>
-      <c r="E61" s="94"/>
-      <c r="F61" s="94"/>
-      <c r="G61" s="94"/>
-      <c r="H61" s="94"/>
-    </row>
-    <row r="62" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A62" s="95"/>
-      <c r="B62" s="35"/>
-      <c r="C62" s="35"/>
-      <c r="D62" s="35"/>
-      <c r="E62" s="35"/>
-      <c r="F62" s="35"/>
-      <c r="H62" s="35"/>
-    </row>
-    <row r="63" spans="1:34" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="124" t="s">
+      <c r="B63" s="120"/>
+      <c r="C63" s="94"/>
+      <c r="D63" s="94"/>
+      <c r="E63" s="94"/>
+      <c r="F63" s="94"/>
+      <c r="G63" s="94"/>
+      <c r="H63" s="94"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="95"/>
+      <c r="B64" s="35"/>
+      <c r="C64" s="35"/>
+      <c r="D64" s="35"/>
+      <c r="E64" s="35"/>
+      <c r="F64" s="35"/>
+      <c r="H64" s="35"/>
+    </row>
+    <row r="65" spans="1:34" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="124" t="s">
         <v>170</v>
       </c>
-      <c r="B63" s="124"/>
-      <c r="C63" s="124"/>
-      <c r="D63" s="124"/>
-      <c r="E63" s="124"/>
-      <c r="F63" s="124"/>
-      <c r="G63" s="124"/>
-      <c r="H63" s="124"/>
-      <c r="I63" s="54"/>
-      <c r="J63" s="54"/>
-      <c r="K63" s="54"/>
-      <c r="L63" s="54"/>
-      <c r="M63" s="55"/>
-      <c r="N63" s="55"/>
-      <c r="O63" s="55"/>
-      <c r="P63" s="55"/>
-      <c r="Q63" s="55"/>
-      <c r="R63" s="35"/>
-      <c r="S63" s="35"/>
-      <c r="T63" s="35"/>
-      <c r="U63" s="35"/>
-      <c r="V63" s="35"/>
-      <c r="W63" s="35"/>
-      <c r="X63" s="35"/>
-      <c r="Y63" s="35"/>
-      <c r="Z63" s="35"/>
-      <c r="AA63" s="35"/>
-      <c r="AB63" s="35"/>
-      <c r="AC63" s="35"/>
-      <c r="AD63" s="35"/>
-      <c r="AE63" s="35"/>
-      <c r="AF63" s="35"/>
-      <c r="AG63" s="35"/>
-      <c r="AH63" s="35"/>
-    </row>
-    <row r="64" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A64" s="125" t="s">
-        <v>172</v>
-      </c>
-      <c r="B64" s="125"/>
-      <c r="C64" s="125"/>
-      <c r="D64" s="125"/>
-      <c r="E64" s="125"/>
-      <c r="F64" s="125"/>
-      <c r="G64" s="125"/>
-      <c r="H64" s="125"/>
-      <c r="I64" s="54"/>
-      <c r="J64" s="54"/>
-      <c r="K64" s="54"/>
-      <c r="L64" s="54"/>
-      <c r="M64" s="55"/>
-      <c r="N64" s="55"/>
-      <c r="O64" s="55"/>
-      <c r="P64" s="55"/>
-      <c r="Q64" s="55"/>
-      <c r="R64" s="35"/>
-      <c r="S64" s="35"/>
-      <c r="T64" s="35"/>
-      <c r="U64" s="35"/>
-      <c r="V64" s="35"/>
-      <c r="W64" s="35"/>
-      <c r="X64" s="35"/>
-      <c r="Y64" s="35"/>
-      <c r="Z64" s="35"/>
-      <c r="AA64" s="35"/>
-      <c r="AB64" s="35"/>
-      <c r="AC64" s="35"/>
-      <c r="AD64" s="35"/>
-      <c r="AE64" s="35"/>
-      <c r="AF64" s="35"/>
-      <c r="AG64" s="35"/>
-      <c r="AH64" s="35"/>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A65" s="126" t="s">
+      <c r="B65" s="124"/>
+      <c r="C65" s="124"/>
+      <c r="D65" s="124"/>
+      <c r="E65" s="124"/>
+      <c r="F65" s="124"/>
+      <c r="G65" s="124"/>
+      <c r="H65" s="124"/>
+      <c r="I65" s="54"/>
+      <c r="J65" s="54"/>
+      <c r="K65" s="54"/>
+      <c r="L65" s="54"/>
+      <c r="M65" s="55"/>
+      <c r="N65" s="55"/>
+      <c r="O65" s="55"/>
+      <c r="P65" s="55"/>
+      <c r="Q65" s="55"/>
+      <c r="R65" s="35"/>
+      <c r="S65" s="35"/>
+      <c r="T65" s="35"/>
+      <c r="U65" s="35"/>
+      <c r="V65" s="35"/>
+      <c r="W65" s="35"/>
+      <c r="X65" s="35"/>
+      <c r="Y65" s="35"/>
+      <c r="Z65" s="35"/>
+      <c r="AA65" s="35"/>
+      <c r="AB65" s="35"/>
+      <c r="AC65" s="35"/>
+      <c r="AD65" s="35"/>
+      <c r="AE65" s="35"/>
+      <c r="AF65" s="35"/>
+      <c r="AG65" s="35"/>
+      <c r="AH65" s="35"/>
+    </row>
+    <row r="66" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A66" s="128" t="s">
+        <v>177</v>
+      </c>
+      <c r="B66" s="128"/>
+      <c r="C66" s="128"/>
+      <c r="D66" s="128"/>
+      <c r="E66" s="128"/>
+      <c r="F66" s="128"/>
+      <c r="G66" s="128"/>
+      <c r="H66" s="128"/>
+      <c r="I66" s="54"/>
+      <c r="J66" s="54"/>
+      <c r="K66" s="54"/>
+      <c r="L66" s="54"/>
+      <c r="M66" s="55"/>
+      <c r="N66" s="55"/>
+      <c r="O66" s="55"/>
+      <c r="P66" s="55"/>
+      <c r="Q66" s="55"/>
+      <c r="R66" s="35"/>
+      <c r="S66" s="35"/>
+      <c r="T66" s="35"/>
+      <c r="U66" s="35"/>
+      <c r="V66" s="35"/>
+      <c r="W66" s="35"/>
+      <c r="X66" s="35"/>
+      <c r="Y66" s="35"/>
+      <c r="Z66" s="35"/>
+      <c r="AA66" s="35"/>
+      <c r="AB66" s="35"/>
+      <c r="AC66" s="35"/>
+      <c r="AD66" s="35"/>
+      <c r="AE66" s="35"/>
+      <c r="AF66" s="35"/>
+      <c r="AG66" s="35"/>
+      <c r="AH66" s="35"/>
+    </row>
+    <row r="67" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A67" s="127" t="s">
+        <v>176</v>
+      </c>
+      <c r="B67" s="127"/>
+      <c r="C67" s="127"/>
+      <c r="D67" s="127"/>
+      <c r="E67" s="127"/>
+      <c r="F67" s="127"/>
+      <c r="G67" s="127"/>
+      <c r="H67" s="127"/>
+      <c r="I67" s="54"/>
+      <c r="J67" s="54"/>
+      <c r="K67" s="54"/>
+      <c r="L67" s="54"/>
+      <c r="M67" s="55"/>
+      <c r="N67" s="55"/>
+      <c r="O67" s="55"/>
+      <c r="P67" s="55"/>
+      <c r="Q67" s="55"/>
+      <c r="R67" s="35"/>
+      <c r="S67" s="35"/>
+      <c r="T67" s="35"/>
+      <c r="U67" s="35"/>
+      <c r="V67" s="35"/>
+      <c r="W67" s="35"/>
+      <c r="X67" s="35"/>
+      <c r="Y67" s="35"/>
+      <c r="Z67" s="35"/>
+      <c r="AA67" s="35"/>
+      <c r="AB67" s="35"/>
+      <c r="AC67" s="35"/>
+      <c r="AD67" s="35"/>
+      <c r="AE67" s="35"/>
+      <c r="AF67" s="35"/>
+      <c r="AG67" s="35"/>
+      <c r="AH67" s="35"/>
+    </row>
+    <row r="68" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A68" s="125" t="s">
         <v>169</v>
       </c>
-      <c r="B65" s="127"/>
-      <c r="C65" s="127"/>
-      <c r="D65" s="127"/>
-      <c r="E65" s="127"/>
-      <c r="F65" s="127"/>
-      <c r="G65" s="127"/>
-      <c r="H65" s="127"/>
-      <c r="I65" s="57"/>
-      <c r="J65" s="57"/>
-      <c r="K65" s="57"/>
-      <c r="L65" s="57"/>
-      <c r="M65" s="41"/>
-      <c r="N65" s="41"/>
-      <c r="O65" s="41"/>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A66" s="59"/>
-      <c r="B66" s="59"/>
-      <c r="C66" s="59"/>
-      <c r="D66" s="59"/>
-      <c r="E66" s="59"/>
-      <c r="F66" s="59"/>
-      <c r="G66" s="59"/>
-      <c r="H66" s="59"/>
-      <c r="I66" s="41"/>
-      <c r="J66" s="41"/>
-      <c r="K66" s="41"/>
-      <c r="L66" s="41"/>
-      <c r="M66" s="41"/>
-      <c r="N66" s="41"/>
-      <c r="O66" s="41"/>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A67" s="59"/>
-      <c r="B67" s="59"/>
-      <c r="C67" s="59"/>
-      <c r="D67" s="59"/>
-      <c r="E67" s="59"/>
-      <c r="F67" s="59"/>
-      <c r="G67" s="59"/>
-      <c r="H67" s="59"/>
-      <c r="I67" s="41"/>
-      <c r="J67" s="41"/>
-      <c r="K67" s="41"/>
-      <c r="L67" s="41"/>
-      <c r="M67" s="41"/>
-      <c r="N67" s="41"/>
-      <c r="O67" s="41"/>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A68" s="58" t="s">
-        <v>5</v>
-      </c>
-      <c r="B68" s="78" t="s">
-        <v>117</v>
-      </c>
-      <c r="C68" s="104" t="s">
-        <v>117</v>
-      </c>
-      <c r="D68" s="104"/>
-      <c r="E68" s="35"/>
-      <c r="F68" s="104"/>
-      <c r="G68" s="104"/>
-      <c r="H68" s="78"/>
-      <c r="I68" s="72"/>
-      <c r="J68" s="72"/>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B68" s="126"/>
+      <c r="C68" s="126"/>
+      <c r="D68" s="126"/>
+      <c r="E68" s="126"/>
+      <c r="F68" s="126"/>
+      <c r="G68" s="126"/>
+      <c r="H68" s="126"/>
+      <c r="I68" s="57"/>
+      <c r="J68" s="57"/>
+      <c r="K68" s="57"/>
+      <c r="L68" s="57"/>
+      <c r="M68" s="41"/>
+      <c r="N68" s="41"/>
+      <c r="O68" s="41"/>
+    </row>
+    <row r="69" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A69" s="59"/>
-      <c r="B69" s="99" t="s">
-        <v>168</v>
-      </c>
-      <c r="C69" s="104" t="s">
-        <v>1</v>
-      </c>
-      <c r="D69" s="104"/>
-      <c r="E69" s="35"/>
-      <c r="F69" s="104"/>
-      <c r="G69" s="104"/>
-      <c r="H69" s="78"/>
+      <c r="B69" s="59"/>
+      <c r="C69" s="59"/>
+      <c r="D69" s="59"/>
+      <c r="E69" s="59"/>
+      <c r="F69" s="59"/>
+      <c r="G69" s="59"/>
+      <c r="H69" s="59"/>
       <c r="I69" s="41"/>
       <c r="J69" s="41"/>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K69" s="41"/>
+      <c r="L69" s="41"/>
+      <c r="M69" s="41"/>
+      <c r="N69" s="41"/>
+      <c r="O69" s="41"/>
+    </row>
+    <row r="70" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A70" s="59"/>
       <c r="B70" s="59"/>
       <c r="C70" s="59"/>
@@ -8712,66 +8750,118 @@
       <c r="N70" s="41"/>
       <c r="O70" s="41"/>
     </row>
-    <row r="71" spans="1:15" s="85" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="118" t="s">
+    <row r="71" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A71" s="58" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71" s="78" t="s">
+        <v>117</v>
+      </c>
+      <c r="C71" s="104" t="s">
+        <v>117</v>
+      </c>
+      <c r="D71" s="104"/>
+      <c r="E71" s="35"/>
+      <c r="F71" s="104"/>
+      <c r="G71" s="104"/>
+      <c r="H71" s="78"/>
+      <c r="I71" s="72"/>
+      <c r="J71" s="72"/>
+    </row>
+    <row r="72" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A72" s="59"/>
+      <c r="B72" s="99" t="s">
+        <v>168</v>
+      </c>
+      <c r="C72" s="104" t="s">
+        <v>1</v>
+      </c>
+      <c r="D72" s="104"/>
+      <c r="E72" s="35"/>
+      <c r="F72" s="104"/>
+      <c r="G72" s="104"/>
+      <c r="H72" s="78"/>
+      <c r="I72" s="41"/>
+      <c r="J72" s="41"/>
+    </row>
+    <row r="73" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A73" s="59"/>
+      <c r="B73" s="59"/>
+      <c r="C73" s="59"/>
+      <c r="D73" s="59"/>
+      <c r="E73" s="59"/>
+      <c r="F73" s="59"/>
+      <c r="G73" s="59"/>
+      <c r="H73" s="59"/>
+      <c r="I73" s="41"/>
+      <c r="J73" s="41"/>
+      <c r="K73" s="41"/>
+      <c r="L73" s="41"/>
+      <c r="M73" s="41"/>
+      <c r="N73" s="41"/>
+      <c r="O73" s="41"/>
+    </row>
+    <row r="74" spans="1:34" s="85" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="118" t="s">
         <v>153</v>
       </c>
-      <c r="B71" s="118"/>
-      <c r="C71" s="118"/>
-      <c r="D71" s="118"/>
-      <c r="E71" s="118"/>
-      <c r="F71" s="118"/>
-      <c r="G71" s="118"/>
-      <c r="H71" s="118"/>
-      <c r="I71" s="42"/>
-      <c r="J71" s="42"/>
-      <c r="K71" s="42"/>
-      <c r="L71" s="42"/>
-      <c r="M71" s="84"/>
-      <c r="N71" s="84"/>
-      <c r="O71" s="84"/>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A72" s="35"/>
-      <c r="B72" s="35"/>
-      <c r="C72" s="35"/>
-      <c r="D72" s="35"/>
-      <c r="E72" s="35"/>
-      <c r="F72" s="35"/>
-    </row>
-    <row r="86" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E86" s="36" t="s">
+      <c r="B74" s="118"/>
+      <c r="C74" s="118"/>
+      <c r="D74" s="118"/>
+      <c r="E74" s="118"/>
+      <c r="F74" s="118"/>
+      <c r="G74" s="118"/>
+      <c r="H74" s="118"/>
+      <c r="I74" s="42"/>
+      <c r="J74" s="42"/>
+      <c r="K74" s="42"/>
+      <c r="L74" s="42"/>
+      <c r="M74" s="84"/>
+      <c r="N74" s="84"/>
+      <c r="O74" s="84"/>
+    </row>
+    <row r="75" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A75" s="35"/>
+      <c r="B75" s="35"/>
+      <c r="C75" s="35"/>
+      <c r="D75" s="35"/>
+      <c r="E75" s="35"/>
+      <c r="F75" s="35"/>
+    </row>
+    <row r="89" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E89" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="F86" s="36" t="s">
+      <c r="F89" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="G86" s="35" t="s">
+      <c r="G89" s="35" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="A71:H71"/>
-    <mergeCell ref="A61:B61"/>
+  <mergeCells count="12">
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="A74:H74"/>
+    <mergeCell ref="A63:B63"/>
     <mergeCell ref="A12:H12"/>
-    <mergeCell ref="A37:H37"/>
-    <mergeCell ref="A63:H63"/>
-    <mergeCell ref="A64:H64"/>
+    <mergeCell ref="A39:H39"/>
     <mergeCell ref="A65:H65"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="A66:H66"/>
+    <mergeCell ref="A68:H68"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="A67:H67"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup scale="35" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="78" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Negrita"&amp;8&amp;U
 RECOPILACIÓN DE NORMAS PARA SERVICIOS FINANCIEROS&amp;R&amp;"Times New Roman,Negrita Cursiva"&amp;7AUTORIDAD DE SUPERVISIÓN DEL SISTEMA FINANCIERO</oddHeader>
     <oddFooter>&amp;L&amp;"Times New Roman,Cursiva"&amp;8&amp;K0000FFControl de versiones&amp;K01+000
-Circular ASFI/731/2022 (última)
+Circular ASFI/812/2024 (última)
 &amp;R&amp;"Times New Roman,Normal"&amp;8Libro 5°
 Título II
 Capítulo III

</xml_diff>